<commit_message>
better representation of data model
</commit_message>
<xml_diff>
--- a/program_config.xlsx
+++ b/program_config.xlsx
@@ -536,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,12 +567,52 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>localisation</t>
+          <t>country</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>industrie</t>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>product_type_1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>product_type_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>product_type_3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>line_of_business</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>industry</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>sic_code</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>include</t>
         </is>
       </c>
     </row>
@@ -589,6 +629,14 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -603,10 +651,18 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -623,10 +679,18 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>